<commit_message>
add project2 - not finished
</commit_message>
<xml_diff>
--- a/project/data/aram_portfolio.xlsx
+++ b/project/data/aram_portfolio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Documents/advanced_stochastic/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05FB3E6-1B87-BC4B-9243-FD2CB0D62C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5883C6B5-AAE7-3847-AB82-B18A8B0FC238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34240" windowHeight="18760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34240" windowHeight="18760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="سهام" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="203">
   <si>
     <t>صندوق سرمایه‌گذاری شاخصی آرام مفید</t>
   </si>
@@ -521,24 +521,6 @@
     <t>holding</t>
   </si>
   <si>
-    <t>call_symbol</t>
-  </si>
-  <si>
-    <t>call_mat_date</t>
-  </si>
-  <si>
-    <t>call_strike</t>
-  </si>
-  <si>
-    <t>put_symbol</t>
-  </si>
-  <si>
-    <t>put_mat_date</t>
-  </si>
-  <si>
-    <t>put_strike</t>
-  </si>
-  <si>
     <t>خودرو</t>
   </si>
   <si>
@@ -648,6 +630,24 @@
   </si>
   <si>
     <t>طفلا7022</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>strike</t>
+  </si>
+  <si>
+    <t>maturity_date</t>
+  </si>
+  <si>
+    <t>option_symbol</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,6 +790,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,11 +802,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,15 +1120,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Y81"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView rightToLeft="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="32.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="1" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="1" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1" style="1" customWidth="1"/>
@@ -1158,250 +1157,250 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
     </row>
     <row r="3" spans="1:25" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
     </row>
     <row r="4" spans="1:25" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
     </row>
     <row r="6" spans="1:25" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="18" t="s">
+      <c r="T6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="18" t="s">
+      <c r="U6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="V6" s="18" t="s">
+      <c r="V6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="W6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="X6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Y6" s="18" t="s">
+      <c r="Y6" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="21">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="17" t="s">
+      <c r="Q7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="17" t="s">
+      <c r="S7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="17" t="s">
+      <c r="U7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="17" t="s">
+      <c r="W7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="Y7" s="17" t="s">
+      <c r="Y7" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="21">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="18" t="s">
+      <c r="U8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="W8" s="18" t="s">
+      <c r="W8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="Y8" s="18" t="s">
+      <c r="Y8" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="21">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="6">
@@ -1453,7 +1452,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="21">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="6">
@@ -1505,7 +1504,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="21">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="6">
@@ -1557,7 +1556,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="21">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="6">
@@ -1713,7 +1712,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="21">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="6">
@@ -1765,7 +1764,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="21">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="6">
@@ -1869,7 +1868,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="21">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="18" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="6">
@@ -2961,7 +2960,7 @@
       </c>
     </row>
     <row r="39" spans="1:25" ht="21">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="6">
@@ -3065,7 +3064,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" ht="21">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C41" s="6">
@@ -3793,7 +3792,7 @@
       </c>
     </row>
     <row r="55" spans="1:25">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="19" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="6">
@@ -4001,7 +4000,7 @@
       </c>
     </row>
     <row r="59" spans="1:25" ht="21">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C59" s="6">
@@ -5116,11 +5115,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="A4:Y4"/>
     <mergeCell ref="A3:Y3"/>
     <mergeCell ref="A2:Y2"/>
@@ -5137,6 +5131,11 @@
     <mergeCell ref="M8"/>
     <mergeCell ref="O8"/>
     <mergeCell ref="M7:O7"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5170,96 +5169,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:11" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="6" spans="1:11" ht="21">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5411,34 +5410,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="20" t="s">
         <v>108</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -5446,22 +5445,22 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="21"/>
       <c r="E6" s="12" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5506,298 +5505,459 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E21841-C107-AA42-97DE-3B868F6E52A5}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="B2" s="23">
+        <v>38372289</v>
+      </c>
+      <c r="C2" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="21">
-        <v>1.41E-2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>168</v>
       </c>
       <c r="E2">
         <v>3000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="23">
+        <v>38372289</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3">
+        <v>3000</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="23">
+        <v>27555013</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4">
+        <v>2942</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="23">
+        <v>27555013</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5">
+        <v>2942</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="23">
+        <v>30935774</v>
+      </c>
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="E6">
+        <v>2797</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="23">
+        <v>30935774</v>
+      </c>
+      <c r="C7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7">
+        <v>2797</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="21">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B8" s="23">
+        <v>57146213</v>
+      </c>
+      <c r="C8" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="E3">
-        <v>2942</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="E8">
+        <v>4370</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="23">
+        <v>57146213</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9">
+        <v>4370</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="23">
+        <v>32895084</v>
+      </c>
+      <c r="C10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" s="17">
+        <v>14000</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="23">
+        <v>32895084</v>
+      </c>
+      <c r="C11" t="s">
         <v>179</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="D11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11">
+        <v>14000</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="23">
+        <v>16768904</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="17">
+        <v>15000</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="23">
+        <v>16768904</v>
+      </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="17">
+        <v>15000</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="23">
+        <v>38230557</v>
+      </c>
+      <c r="C14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="17">
+        <v>6500</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="23">
+        <v>38230557</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="17">
+        <v>6500</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="23">
+        <v>27220678</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="17">
+        <v>2000</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="23">
+        <v>27220678</v>
+      </c>
+      <c r="C17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="17">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="23">
+        <v>251234944</v>
+      </c>
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="17">
+        <v>1700</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="23">
+        <v>251234944</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1700</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="23">
+        <v>116811416</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="H3">
-        <v>2942</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="21">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4">
-        <v>2797</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4">
-        <v>2797</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="21">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5">
-        <v>4370</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5">
-        <v>4370</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="21">
-        <v>3.3500000000000002E-2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E6" s="20">
-        <v>14000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="H6">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="21">
-        <v>2.64E-2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="E20" s="17">
+        <v>2484</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="23">
+        <v>116811416</v>
+      </c>
+      <c r="C21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="E7" s="20">
-        <v>15000</v>
-      </c>
-      <c r="F7" t="s">
-        <v>188</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="20">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="21">
-        <v>2.3199999999999998E-2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="E8" s="20">
-        <v>6500</v>
-      </c>
-      <c r="F8" t="s">
-        <v>192</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="H8" s="20">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="21">
-        <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="20">
-        <v>2000</v>
-      </c>
-      <c r="F9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" s="21">
-        <v>3.7400000000000003E-2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="20">
-        <v>1700</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E21" s="17">
+        <v>2484</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="H10" s="20">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="23">
-        <v>7.6200000000000004E-2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>201</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E11" s="20">
-        <v>2484</v>
-      </c>
-      <c r="F11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="H11" s="20">
-        <v>2484</v>
       </c>
     </row>
   </sheetData>
@@ -5841,150 +6001,150 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:19" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
     </row>
     <row r="4" spans="1:19" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
     <row r="6" spans="1:19" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="S7" s="21" t="s">
         <v>87</v>
       </c>
     </row>
@@ -6138,11 +6298,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C7"/>
-    <mergeCell ref="E7"/>
-    <mergeCell ref="G7"/>
-    <mergeCell ref="I7"/>
-    <mergeCell ref="C6:I6"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
     <mergeCell ref="A4:S4"/>
@@ -6155,6 +6310,11 @@
     <mergeCell ref="O7"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C7"/>
+    <mergeCell ref="E7"/>
+    <mergeCell ref="G7"/>
+    <mergeCell ref="I7"/>
+    <mergeCell ref="C6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6199,156 +6359,156 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
     </row>
     <row r="4" spans="1:21" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
     <row r="6" spans="1:21" ht="21">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="21">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="S7" s="19" t="s">
+      <c r="S7" s="22" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6546,49 +6706,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="6" spans="1:7" ht="21">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6695,153 +6855,153 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
     </row>
     <row r="4" spans="1:21" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
     <row r="6" spans="1:21" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="S7" s="21" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7838,147 +7998,147 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="24.75" customHeight="1">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="21" t="s">
         <v>135</v>
       </c>
     </row>
@@ -10580,141 +10740,141 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
     </row>
     <row r="3" spans="1:17" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
     </row>
     <row r="4" spans="1:17" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
     </row>
     <row r="6" spans="1:17" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="21" t="s">
         <v>136</v>
       </c>
     </row>
@@ -13640,171 +13800,171 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="21">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
+      <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="1:21" ht="21">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
     </row>
     <row r="6" spans="1:21" ht="21">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="T6" s="18" t="s">
+      <c r="T6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="U6" s="18" t="s">
+      <c r="U6" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="21">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="S7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="U7" s="18" t="s">
+      <c r="U7" s="21" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>